<commit_message>
updated Hyperparam to accomadate dropout list
</commit_message>
<xml_diff>
--- a/Hyperparameters_Data.xlsx
+++ b/Hyperparameters_Data.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\acb\GitHub\BuildingLandability\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B7675475-7B51-4735-9D8F-C372DD99A63B}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{04C2AAEE-8760-4590-9D1F-CF60D358E629}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="5520" yWindow="1812" windowWidth="17520" windowHeight="7896" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Hyperparam Accuracies" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="90" uniqueCount="18">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="91" uniqueCount="19">
   <si>
     <t>Neural Net Type</t>
   </si>
@@ -74,6 +74,9 @@
   </si>
   <si>
     <t>binary_crossentropy</t>
+  </si>
+  <si>
+    <t>Batch Norm Booleans</t>
   </si>
 </sst>
 </file>
@@ -420,15 +423,15 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:N20"/>
+  <dimension ref="A1:O20"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B13" workbookViewId="0">
-      <selection activeCell="P16" sqref="P16"/>
+    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
+      <selection activeCell="P5" sqref="P5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
-    <row r="1" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -471,8 +474,11 @@
       <c r="N1" t="s">
         <v>13</v>
       </c>
-    </row>
-    <row r="2" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="O1" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="2" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>14</v>
       </c>
@@ -516,7 +522,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>14</v>
       </c>
@@ -560,7 +566,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>14</v>
       </c>
@@ -604,7 +610,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="5" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>14</v>
       </c>
@@ -648,7 +654,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="6" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>14</v>
       </c>
@@ -692,7 +698,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="7" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
         <v>14</v>
       </c>
@@ -736,7 +742,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="8" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
         <v>14</v>
       </c>
@@ -780,7 +786,7 @@
         <v>0.35539999999999999</v>
       </c>
     </row>
-    <row r="9" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
         <v>14</v>
       </c>
@@ -824,7 +830,7 @@
         <v>0.3553</v>
       </c>
     </row>
-    <row r="10" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
         <v>14</v>
       </c>
@@ -868,7 +874,7 @@
         <v>0.3553</v>
       </c>
     </row>
-    <row r="11" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
         <v>14</v>
       </c>
@@ -912,7 +918,7 @@
         <v>0.3553</v>
       </c>
     </row>
-    <row r="12" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
         <v>14</v>
       </c>
@@ -956,7 +962,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="13" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
         <v>14</v>
       </c>
@@ -1000,7 +1006,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="14" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
         <v>14</v>
       </c>
@@ -1044,7 +1050,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="15" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
         <v>14</v>
       </c>
@@ -1088,7 +1094,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="16" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
         <v>14</v>
       </c>

</xml_diff>

<commit_message>
Updating with hyperparamstudy models
</commit_message>
<xml_diff>
--- a/Hyperparameters_Data.xlsx
+++ b/Hyperparameters_Data.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22730"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22827"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\andre\AppData\Local\Temp\scp46245\home\ubuntu\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\andre\AppData\Local\Temp\scp35127\home\ubuntu\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F93E59A8-DA1F-4284-AC0B-81175CB48B65}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{99D33F8F-6CB7-4EB5-9511-2B5049E78692}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="4464" yWindow="996" windowWidth="17520" windowHeight="8388" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Hyperparam Accuracies" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="134" uniqueCount="27">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="309" uniqueCount="49">
   <si>
     <t>Neural Net Type</t>
   </si>
@@ -91,6 +91,9 @@
     <t>16.0, 32.0, 64.0, 128.0, 256.0</t>
   </si>
   <si>
+    <t>mostly black</t>
+  </si>
+  <si>
     <t>0.1, 0.1</t>
   </si>
   <si>
@@ -100,7 +103,70 @@
     <t>0.1, 0.5</t>
   </si>
   <si>
+    <t>~3000</t>
+  </si>
+  <si>
+    <t>decent, needs more training</t>
+  </si>
+  <si>
     <t>0.3, 0.1</t>
+  </si>
+  <si>
+    <t>not good</t>
+  </si>
+  <si>
+    <t>0.3, 0.3</t>
+  </si>
+  <si>
+    <t>terrible, nearly all black</t>
+  </si>
+  <si>
+    <t>0.3, 0.5</t>
+  </si>
+  <si>
+    <t>0.5, 0.1</t>
+  </si>
+  <si>
+    <t>0.5, 0.3</t>
+  </si>
+  <si>
+    <t>0.5, 0.5</t>
+  </si>
+  <si>
+    <t>0.6, 0.1</t>
+  </si>
+  <si>
+    <t>0.6, 0.3</t>
+  </si>
+  <si>
+    <t>0.6, 0.5</t>
+  </si>
+  <si>
+    <t>0.7, 0.1</t>
+  </si>
+  <si>
+    <t>0.7, 0.3</t>
+  </si>
+  <si>
+    <t>too much high frequency noise, not trained long enough</t>
+  </si>
+  <si>
+    <t>0.7, 0.5</t>
+  </si>
+  <si>
+    <t>step</t>
+  </si>
+  <si>
+    <t>not bad, thinks roads and shadows are landable</t>
+  </si>
+  <si>
+    <t>not too bad, but not good</t>
+  </si>
+  <si>
+    <t>mostly black, loss way too high</t>
+  </si>
+  <si>
+    <t>pretty bad, but learned that roads aren't landable, more training needed</t>
   </si>
 </sst>
 </file>
@@ -447,16 +513,17 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:P26"/>
+  <dimension ref="A1:T49"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B7" workbookViewId="0">
-      <selection activeCell="M27" sqref="M27"/>
+    <sheetView tabSelected="1" topLeftCell="A43" workbookViewId="0">
+      <selection activeCell="N51" sqref="N51"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="15" max="15" width="19.33203125" customWidth="1"/>
     <col min="16" max="16" width="22.5546875" customWidth="1"/>
+    <col min="19" max="19" width="8.88671875" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:16" x14ac:dyDescent="0.3">
@@ -1169,7 +1236,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="17" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
         <v>16</v>
       </c>
@@ -1213,7 +1280,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="18" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A18" t="s">
         <v>16</v>
       </c>
@@ -1257,7 +1324,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="19" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A19" t="s">
         <v>16</v>
       </c>
@@ -1301,7 +1368,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="20" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A20" t="s">
         <v>16</v>
       </c>
@@ -1345,7 +1412,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="21" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A21" t="s">
         <v>16</v>
       </c>
@@ -1395,7 +1462,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="22" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A22" t="s">
         <v>16</v>
       </c>
@@ -1444,8 +1511,17 @@
       <c r="P22" t="s">
         <v>22</v>
       </c>
-    </row>
-    <row r="23" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="R22">
+        <v>0.66390000000000005</v>
+      </c>
+      <c r="S22">
+        <v>55648</v>
+      </c>
+      <c r="T22" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="23" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A23" t="s">
         <v>16</v>
       </c>
@@ -1465,7 +1541,7 @@
         <v>0</v>
       </c>
       <c r="G23" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="H23">
         <v>32</v>
@@ -1495,7 +1571,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="24" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A24" t="s">
         <v>16</v>
       </c>
@@ -1515,7 +1591,7 @@
         <v>0</v>
       </c>
       <c r="G24" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="H24">
         <v>32</v>
@@ -1545,7 +1621,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="25" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A25" t="s">
         <v>16</v>
       </c>
@@ -1565,7 +1641,7 @@
         <v>0</v>
       </c>
       <c r="G25" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="H25">
         <v>32</v>
@@ -1594,8 +1670,17 @@
       <c r="P25" t="s">
         <v>22</v>
       </c>
-    </row>
-    <row r="26" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="R25">
+        <v>0.57550000000000001</v>
+      </c>
+      <c r="S25" t="s">
+        <v>27</v>
+      </c>
+      <c r="T25" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="26" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A26" t="s">
         <v>16</v>
       </c>
@@ -1615,7 +1700,7 @@
         <v>0</v>
       </c>
       <c r="G26" t="s">
-        <v>26</v>
+        <v>29</v>
       </c>
       <c r="H26">
         <v>32</v>
@@ -1642,6 +1727,1246 @@
         <v>21</v>
       </c>
       <c r="P26" t="s">
+        <v>22</v>
+      </c>
+      <c r="R26">
+        <v>0.58720000000000006</v>
+      </c>
+      <c r="S26" t="s">
+        <v>27</v>
+      </c>
+      <c r="T26" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="27" spans="1:20" x14ac:dyDescent="0.3">
+      <c r="A27" t="s">
+        <v>16</v>
+      </c>
+      <c r="B27">
+        <v>9</v>
+      </c>
+      <c r="C27">
+        <v>1E-3</v>
+      </c>
+      <c r="D27">
+        <v>0</v>
+      </c>
+      <c r="E27" t="s">
+        <v>17</v>
+      </c>
+      <c r="F27">
+        <v>0</v>
+      </c>
+      <c r="G27" t="s">
+        <v>31</v>
+      </c>
+      <c r="H27">
+        <v>32</v>
+      </c>
+      <c r="I27">
+        <v>70</v>
+      </c>
+      <c r="J27" t="s">
+        <v>18</v>
+      </c>
+      <c r="K27" t="s">
+        <v>19</v>
+      </c>
+      <c r="L27">
+        <v>0.94570833444595337</v>
+      </c>
+      <c r="M27">
+        <v>0.86745971441268921</v>
+      </c>
+      <c r="N27">
+        <v>0.36299999999999999</v>
+      </c>
+      <c r="O27" t="s">
+        <v>21</v>
+      </c>
+      <c r="P27" t="s">
+        <v>22</v>
+      </c>
+      <c r="R27">
+        <v>0.65610000000000002</v>
+      </c>
+      <c r="S27">
+        <v>22000</v>
+      </c>
+      <c r="T27" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="28" spans="1:20" x14ac:dyDescent="0.3">
+      <c r="A28" t="s">
+        <v>16</v>
+      </c>
+      <c r="B28">
+        <v>9</v>
+      </c>
+      <c r="C28">
+        <v>1E-3</v>
+      </c>
+      <c r="D28">
+        <v>0</v>
+      </c>
+      <c r="E28" t="s">
+        <v>17</v>
+      </c>
+      <c r="F28">
+        <v>0</v>
+      </c>
+      <c r="G28" t="s">
+        <v>33</v>
+      </c>
+      <c r="H28">
+        <v>32</v>
+      </c>
+      <c r="I28">
+        <v>70</v>
+      </c>
+      <c r="J28" t="s">
+        <v>18</v>
+      </c>
+      <c r="K28" t="s">
+        <v>19</v>
+      </c>
+      <c r="L28">
+        <v>0.94101190567016602</v>
+      </c>
+      <c r="M28">
+        <v>0.87109249830245972</v>
+      </c>
+      <c r="N28">
+        <v>0.374</v>
+      </c>
+      <c r="O28" t="s">
+        <v>21</v>
+      </c>
+      <c r="P28" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="29" spans="1:20" x14ac:dyDescent="0.3">
+      <c r="A29" t="s">
+        <v>16</v>
+      </c>
+      <c r="B29">
+        <v>9</v>
+      </c>
+      <c r="C29">
+        <v>1E-3</v>
+      </c>
+      <c r="D29">
+        <v>0</v>
+      </c>
+      <c r="E29" t="s">
+        <v>17</v>
+      </c>
+      <c r="F29">
+        <v>0</v>
+      </c>
+      <c r="G29" t="s">
+        <v>34</v>
+      </c>
+      <c r="H29">
+        <v>32</v>
+      </c>
+      <c r="I29">
+        <v>70</v>
+      </c>
+      <c r="J29" t="s">
+        <v>18</v>
+      </c>
+      <c r="K29" t="s">
+        <v>19</v>
+      </c>
+      <c r="L29">
+        <v>0.90652602910995483</v>
+      </c>
+      <c r="M29">
+        <v>0.86988288164138794</v>
+      </c>
+      <c r="N29">
+        <v>0.35589999999999999</v>
+      </c>
+      <c r="O29" t="s">
+        <v>21</v>
+      </c>
+      <c r="P29" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="30" spans="1:20" x14ac:dyDescent="0.3">
+      <c r="A30" t="s">
+        <v>16</v>
+      </c>
+      <c r="B30">
+        <v>9</v>
+      </c>
+      <c r="C30">
+        <v>1E-3</v>
+      </c>
+      <c r="D30">
+        <v>0</v>
+      </c>
+      <c r="E30" t="s">
+        <v>17</v>
+      </c>
+      <c r="F30">
+        <v>0</v>
+      </c>
+      <c r="G30" t="s">
+        <v>35</v>
+      </c>
+      <c r="H30">
+        <v>32</v>
+      </c>
+      <c r="I30">
+        <v>70</v>
+      </c>
+      <c r="J30" t="s">
+        <v>18</v>
+      </c>
+      <c r="K30" t="s">
+        <v>19</v>
+      </c>
+      <c r="L30">
+        <v>0.89387792348861694</v>
+      </c>
+      <c r="M30">
+        <v>0.86664044857025146</v>
+      </c>
+      <c r="N30">
+        <v>0.35599999999999998</v>
+      </c>
+      <c r="O30" t="s">
+        <v>21</v>
+      </c>
+      <c r="P30" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="31" spans="1:20" x14ac:dyDescent="0.3">
+      <c r="A31" t="s">
+        <v>16</v>
+      </c>
+      <c r="B31">
+        <v>9</v>
+      </c>
+      <c r="C31">
+        <v>1E-3</v>
+      </c>
+      <c r="D31">
+        <v>0</v>
+      </c>
+      <c r="E31" t="s">
+        <v>17</v>
+      </c>
+      <c r="F31">
+        <v>0</v>
+      </c>
+      <c r="G31" t="s">
+        <v>36</v>
+      </c>
+      <c r="H31">
+        <v>32</v>
+      </c>
+      <c r="I31">
+        <v>70</v>
+      </c>
+      <c r="J31" t="s">
+        <v>18</v>
+      </c>
+      <c r="K31" t="s">
+        <v>19</v>
+      </c>
+      <c r="L31">
+        <v>0.87376844882965088</v>
+      </c>
+      <c r="M31">
+        <v>0.85305732488632202</v>
+      </c>
+      <c r="N31">
+        <v>0.36159999999999998</v>
+      </c>
+      <c r="O31" t="s">
+        <v>21</v>
+      </c>
+      <c r="P31" t="s">
+        <v>22</v>
+      </c>
+      <c r="R31">
+        <v>0.65010000000000001</v>
+      </c>
+      <c r="S31">
+        <v>6037</v>
+      </c>
+      <c r="T31" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="32" spans="1:20" x14ac:dyDescent="0.3">
+      <c r="A32" t="s">
+        <v>16</v>
+      </c>
+      <c r="B32">
+        <v>9</v>
+      </c>
+      <c r="C32">
+        <v>1E-3</v>
+      </c>
+      <c r="D32">
+        <v>0</v>
+      </c>
+      <c r="E32" t="s">
+        <v>17</v>
+      </c>
+      <c r="F32">
+        <v>0</v>
+      </c>
+      <c r="G32" t="s">
+        <v>37</v>
+      </c>
+      <c r="H32">
+        <v>32</v>
+      </c>
+      <c r="I32">
+        <v>70</v>
+      </c>
+      <c r="J32" t="s">
+        <v>18</v>
+      </c>
+      <c r="K32" t="s">
+        <v>19</v>
+      </c>
+      <c r="L32">
+        <v>0.87546622753143311</v>
+      </c>
+      <c r="M32">
+        <v>0.85517746210098267</v>
+      </c>
+      <c r="N32">
+        <v>0.3553</v>
+      </c>
+      <c r="O32" t="s">
+        <v>21</v>
+      </c>
+      <c r="P32" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="33" spans="1:20" x14ac:dyDescent="0.3">
+      <c r="A33" t="s">
+        <v>16</v>
+      </c>
+      <c r="B33">
+        <v>9</v>
+      </c>
+      <c r="C33">
+        <v>1E-3</v>
+      </c>
+      <c r="D33">
+        <v>0</v>
+      </c>
+      <c r="E33" t="s">
+        <v>17</v>
+      </c>
+      <c r="F33">
+        <v>0</v>
+      </c>
+      <c r="G33" t="s">
+        <v>38</v>
+      </c>
+      <c r="H33">
+        <v>32</v>
+      </c>
+      <c r="I33">
+        <v>70</v>
+      </c>
+      <c r="J33" t="s">
+        <v>18</v>
+      </c>
+      <c r="K33" t="s">
+        <v>19</v>
+      </c>
+      <c r="L33">
+        <v>0.85126978158950806</v>
+      </c>
+      <c r="M33">
+        <v>0.83898669481277466</v>
+      </c>
+      <c r="N33">
+        <v>0.35539999999999999</v>
+      </c>
+      <c r="O33" t="s">
+        <v>21</v>
+      </c>
+      <c r="P33" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="34" spans="1:20" x14ac:dyDescent="0.3">
+      <c r="A34" t="s">
+        <v>16</v>
+      </c>
+      <c r="B34">
+        <v>9</v>
+      </c>
+      <c r="C34">
+        <v>1E-3</v>
+      </c>
+      <c r="D34">
+        <v>0</v>
+      </c>
+      <c r="E34" t="s">
+        <v>17</v>
+      </c>
+      <c r="F34">
+        <v>0</v>
+      </c>
+      <c r="G34" t="s">
+        <v>39</v>
+      </c>
+      <c r="H34">
+        <v>32</v>
+      </c>
+      <c r="I34">
+        <v>70</v>
+      </c>
+      <c r="J34" t="s">
+        <v>18</v>
+      </c>
+      <c r="K34" t="s">
+        <v>19</v>
+      </c>
+      <c r="L34">
+        <v>0.86656087636947632</v>
+      </c>
+      <c r="M34">
+        <v>0.84900212287902832</v>
+      </c>
+      <c r="N34">
+        <v>0.35849999999999999</v>
+      </c>
+      <c r="O34" t="s">
+        <v>21</v>
+      </c>
+      <c r="P34" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="35" spans="1:20" x14ac:dyDescent="0.3">
+      <c r="A35" t="s">
+        <v>16</v>
+      </c>
+      <c r="B35">
+        <v>9</v>
+      </c>
+      <c r="C35">
+        <v>1E-3</v>
+      </c>
+      <c r="D35">
+        <v>0</v>
+      </c>
+      <c r="E35" t="s">
+        <v>17</v>
+      </c>
+      <c r="F35">
+        <v>0</v>
+      </c>
+      <c r="G35" t="s">
+        <v>40</v>
+      </c>
+      <c r="H35">
+        <v>32</v>
+      </c>
+      <c r="I35">
+        <v>70</v>
+      </c>
+      <c r="J35" t="s">
+        <v>18</v>
+      </c>
+      <c r="K35" t="s">
+        <v>19</v>
+      </c>
+      <c r="L35">
+        <v>0.71974390745162964</v>
+      </c>
+      <c r="M35">
+        <v>0.70866310596466064</v>
+      </c>
+      <c r="N35">
+        <v>0.3553</v>
+      </c>
+      <c r="O35" t="s">
+        <v>21</v>
+      </c>
+      <c r="P35" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="36" spans="1:20" x14ac:dyDescent="0.3">
+      <c r="A36" t="s">
+        <v>16</v>
+      </c>
+      <c r="B36">
+        <v>9</v>
+      </c>
+      <c r="C36">
+        <v>1E-3</v>
+      </c>
+      <c r="D36">
+        <v>0</v>
+      </c>
+      <c r="E36" t="s">
+        <v>17</v>
+      </c>
+      <c r="F36">
+        <v>0</v>
+      </c>
+      <c r="G36" t="s">
+        <v>41</v>
+      </c>
+      <c r="H36">
+        <v>32</v>
+      </c>
+      <c r="I36">
+        <v>70</v>
+      </c>
+      <c r="J36" t="s">
+        <v>18</v>
+      </c>
+      <c r="K36" t="s">
+        <v>19</v>
+      </c>
+      <c r="L36">
+        <v>0.80988186597824097</v>
+      </c>
+      <c r="M36">
+        <v>0.79963505268096924</v>
+      </c>
+      <c r="N36">
+        <v>0.3553</v>
+      </c>
+      <c r="O36" t="s">
+        <v>21</v>
+      </c>
+      <c r="P36" t="s">
+        <v>22</v>
+      </c>
+      <c r="R36">
+        <v>0.48709999999999998</v>
+      </c>
+      <c r="S36">
+        <v>1066</v>
+      </c>
+      <c r="T36" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="37" spans="1:20" x14ac:dyDescent="0.3">
+      <c r="A37" t="s">
+        <v>16</v>
+      </c>
+      <c r="B37">
+        <v>9</v>
+      </c>
+      <c r="C37">
+        <v>1E-3</v>
+      </c>
+      <c r="D37">
+        <v>0</v>
+      </c>
+      <c r="E37" t="s">
+        <v>17</v>
+      </c>
+      <c r="F37">
+        <v>0</v>
+      </c>
+      <c r="G37" t="s">
+        <v>43</v>
+      </c>
+      <c r="H37">
+        <v>32</v>
+      </c>
+      <c r="I37">
+        <v>70</v>
+      </c>
+      <c r="J37" t="s">
+        <v>18</v>
+      </c>
+      <c r="K37" t="s">
+        <v>19</v>
+      </c>
+      <c r="L37">
+        <v>0.59060502052307129</v>
+      </c>
+      <c r="M37">
+        <v>0.59028464555740356</v>
+      </c>
+      <c r="N37">
+        <v>0.35620000000000002</v>
+      </c>
+      <c r="O37" t="s">
+        <v>21</v>
+      </c>
+      <c r="P37" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="38" spans="1:20" x14ac:dyDescent="0.3">
+      <c r="A38" t="s">
+        <v>16</v>
+      </c>
+      <c r="B38">
+        <v>9</v>
+      </c>
+      <c r="C38">
+        <v>1E-3</v>
+      </c>
+      <c r="D38">
+        <v>0</v>
+      </c>
+      <c r="E38" t="s">
+        <v>17</v>
+      </c>
+      <c r="F38">
+        <v>0</v>
+      </c>
+      <c r="G38" t="s">
+        <v>20</v>
+      </c>
+      <c r="H38">
+        <v>32</v>
+      </c>
+      <c r="I38">
+        <v>2</v>
+      </c>
+      <c r="J38" t="s">
+        <v>18</v>
+      </c>
+      <c r="K38" t="s">
+        <v>19</v>
+      </c>
+      <c r="L38">
+        <v>0.82500076293945313</v>
+      </c>
+      <c r="M38">
+        <v>0.81359732151031494</v>
+      </c>
+      <c r="N38">
+        <v>0.3553</v>
+      </c>
+      <c r="O38" t="s">
+        <v>21</v>
+      </c>
+      <c r="P38" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="39" spans="1:20" x14ac:dyDescent="0.3">
+      <c r="A39" t="s">
+        <v>16</v>
+      </c>
+      <c r="B39">
+        <v>9</v>
+      </c>
+      <c r="C39">
+        <v>1E-3</v>
+      </c>
+      <c r="D39">
+        <v>0.1</v>
+      </c>
+      <c r="E39" t="s">
+        <v>44</v>
+      </c>
+      <c r="F39">
+        <v>0</v>
+      </c>
+      <c r="G39" t="s">
+        <v>29</v>
+      </c>
+      <c r="H39">
+        <v>32</v>
+      </c>
+      <c r="I39">
+        <v>70</v>
+      </c>
+      <c r="J39" t="s">
+        <v>18</v>
+      </c>
+      <c r="K39" t="s">
+        <v>19</v>
+      </c>
+      <c r="L39">
+        <v>0.88386517763137817</v>
+      </c>
+      <c r="M39">
+        <v>0.85690551996231079</v>
+      </c>
+      <c r="N39">
+        <v>0.3553</v>
+      </c>
+      <c r="O39" t="s">
+        <v>21</v>
+      </c>
+      <c r="P39" t="s">
+        <v>22</v>
+      </c>
+      <c r="R39">
+        <v>0.54090000000000005</v>
+      </c>
+      <c r="S39">
+        <v>4866</v>
+      </c>
+      <c r="T39" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="40" spans="1:20" x14ac:dyDescent="0.3">
+      <c r="A40" t="s">
+        <v>16</v>
+      </c>
+      <c r="B40">
+        <v>9</v>
+      </c>
+      <c r="C40">
+        <v>1E-3</v>
+      </c>
+      <c r="D40">
+        <v>0.01</v>
+      </c>
+      <c r="E40" t="s">
+        <v>44</v>
+      </c>
+      <c r="F40">
+        <v>0</v>
+      </c>
+      <c r="G40" t="s">
+        <v>29</v>
+      </c>
+      <c r="H40">
+        <v>32</v>
+      </c>
+      <c r="I40">
+        <v>70</v>
+      </c>
+      <c r="J40" t="s">
+        <v>18</v>
+      </c>
+      <c r="K40" t="s">
+        <v>19</v>
+      </c>
+      <c r="L40">
+        <v>0.87834435701370239</v>
+      </c>
+      <c r="M40">
+        <v>0.85804581642150879</v>
+      </c>
+      <c r="N40">
+        <v>0.3553</v>
+      </c>
+      <c r="O40" t="s">
+        <v>21</v>
+      </c>
+      <c r="P40" t="s">
+        <v>22</v>
+      </c>
+      <c r="R40">
+        <v>0.60089999999999999</v>
+      </c>
+      <c r="S40">
+        <v>5986</v>
+      </c>
+      <c r="T40" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="41" spans="1:20" x14ac:dyDescent="0.3">
+      <c r="A41" t="s">
+        <v>16</v>
+      </c>
+      <c r="B41">
+        <v>9</v>
+      </c>
+      <c r="C41">
+        <v>1E-3</v>
+      </c>
+      <c r="D41">
+        <v>0.1</v>
+      </c>
+      <c r="E41" t="s">
+        <v>17</v>
+      </c>
+      <c r="F41">
+        <v>0</v>
+      </c>
+      <c r="G41" t="s">
+        <v>29</v>
+      </c>
+      <c r="H41">
+        <v>32</v>
+      </c>
+      <c r="I41">
+        <v>70</v>
+      </c>
+      <c r="J41" t="s">
+        <v>18</v>
+      </c>
+      <c r="K41" t="s">
+        <v>19</v>
+      </c>
+      <c r="L41">
+        <v>0.9304581880569458</v>
+      </c>
+      <c r="M41">
+        <v>0.87084388732910156</v>
+      </c>
+      <c r="N41">
+        <v>0.35720000000000002</v>
+      </c>
+      <c r="O41" t="s">
+        <v>21</v>
+      </c>
+      <c r="P41" t="s">
+        <v>22</v>
+      </c>
+      <c r="R41">
+        <v>0.65339999999999998</v>
+      </c>
+      <c r="S41">
+        <v>13364</v>
+      </c>
+      <c r="T41" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="42" spans="1:20" x14ac:dyDescent="0.3">
+      <c r="A42" t="s">
+        <v>16</v>
+      </c>
+      <c r="B42">
+        <v>9</v>
+      </c>
+      <c r="C42">
+        <v>1E-3</v>
+      </c>
+      <c r="D42">
+        <v>0.01</v>
+      </c>
+      <c r="E42" t="s">
+        <v>17</v>
+      </c>
+      <c r="F42">
+        <v>0</v>
+      </c>
+      <c r="G42" t="s">
+        <v>29</v>
+      </c>
+      <c r="H42">
+        <v>32</v>
+      </c>
+      <c r="I42">
+        <v>70</v>
+      </c>
+      <c r="J42" t="s">
+        <v>18</v>
+      </c>
+      <c r="K42" t="s">
+        <v>19</v>
+      </c>
+      <c r="L42">
+        <v>0.96462935209274292</v>
+      </c>
+      <c r="M42">
+        <v>0.87757307291030884</v>
+      </c>
+      <c r="N42">
+        <v>0.36120000000000002</v>
+      </c>
+      <c r="O42" t="s">
+        <v>21</v>
+      </c>
+      <c r="P42" t="s">
+        <v>22</v>
+      </c>
+      <c r="R42">
+        <v>0.65820000000000001</v>
+      </c>
+      <c r="S42">
+        <v>-13000</v>
+      </c>
+      <c r="T42" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="43" spans="1:20" x14ac:dyDescent="0.3">
+      <c r="A43" t="s">
+        <v>16</v>
+      </c>
+      <c r="B43">
+        <v>9</v>
+      </c>
+      <c r="C43">
+        <v>1E-3</v>
+      </c>
+      <c r="D43">
+        <v>0.1</v>
+      </c>
+      <c r="E43" t="s">
+        <v>17</v>
+      </c>
+      <c r="F43">
+        <v>0</v>
+      </c>
+      <c r="G43" t="s">
+        <v>31</v>
+      </c>
+      <c r="H43">
+        <v>32</v>
+      </c>
+      <c r="I43">
+        <v>70</v>
+      </c>
+      <c r="J43" t="s">
+        <v>18</v>
+      </c>
+      <c r="K43" t="s">
+        <v>19</v>
+      </c>
+      <c r="L43">
+        <v>0.9190942645072937</v>
+      </c>
+      <c r="M43">
+        <v>0.85954499244689941</v>
+      </c>
+      <c r="N43">
+        <v>0.37259999999999999</v>
+      </c>
+      <c r="O43" t="s">
+        <v>21</v>
+      </c>
+      <c r="P43" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="44" spans="1:20" x14ac:dyDescent="0.3">
+      <c r="A44" t="s">
+        <v>16</v>
+      </c>
+      <c r="B44">
+        <v>9</v>
+      </c>
+      <c r="C44">
+        <v>1E-3</v>
+      </c>
+      <c r="D44">
+        <v>0.01</v>
+      </c>
+      <c r="E44" t="s">
+        <v>17</v>
+      </c>
+      <c r="F44">
+        <v>0</v>
+      </c>
+      <c r="G44" t="s">
+        <v>31</v>
+      </c>
+      <c r="H44">
+        <v>32</v>
+      </c>
+      <c r="I44">
+        <v>70</v>
+      </c>
+      <c r="J44" t="s">
+        <v>18</v>
+      </c>
+      <c r="K44" t="s">
+        <v>19</v>
+      </c>
+      <c r="L44">
+        <v>0.97406917810440063</v>
+      </c>
+      <c r="M44">
+        <v>0.88373070955276489</v>
+      </c>
+      <c r="N44">
+        <v>0</v>
+      </c>
+      <c r="O44" t="s">
+        <v>21</v>
+      </c>
+      <c r="P44" t="s">
+        <v>22</v>
+      </c>
+      <c r="R44">
+        <v>0.61199999999999999</v>
+      </c>
+      <c r="S44">
+        <v>22000</v>
+      </c>
+      <c r="T44" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="45" spans="1:20" x14ac:dyDescent="0.3">
+      <c r="A45" t="s">
+        <v>16</v>
+      </c>
+      <c r="B45">
+        <v>9</v>
+      </c>
+      <c r="C45">
+        <v>1E-3</v>
+      </c>
+      <c r="D45">
+        <v>0.1</v>
+      </c>
+      <c r="E45" t="s">
+        <v>44</v>
+      </c>
+      <c r="F45">
+        <v>0</v>
+      </c>
+      <c r="G45" t="s">
+        <v>31</v>
+      </c>
+      <c r="H45">
+        <v>32</v>
+      </c>
+      <c r="I45">
+        <v>70</v>
+      </c>
+      <c r="J45" t="s">
+        <v>18</v>
+      </c>
+      <c r="K45" t="s">
+        <v>19</v>
+      </c>
+      <c r="L45">
+        <v>0.8771635890007019</v>
+      </c>
+      <c r="M45">
+        <v>0.85664397478103638</v>
+      </c>
+      <c r="N45">
+        <v>0</v>
+      </c>
+      <c r="O45" t="s">
+        <v>21</v>
+      </c>
+      <c r="P45" t="s">
+        <v>22</v>
+      </c>
+      <c r="R45">
+        <v>0.54090000000000005</v>
+      </c>
+      <c r="S45">
+        <v>4866</v>
+      </c>
+      <c r="T45" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="46" spans="1:20" x14ac:dyDescent="0.3">
+      <c r="A46" t="s">
+        <v>16</v>
+      </c>
+      <c r="B46">
+        <v>9</v>
+      </c>
+      <c r="C46">
+        <v>1E-3</v>
+      </c>
+      <c r="D46">
+        <v>0.01</v>
+      </c>
+      <c r="E46" t="s">
+        <v>44</v>
+      </c>
+      <c r="F46">
+        <v>0</v>
+      </c>
+      <c r="G46" t="s">
+        <v>31</v>
+      </c>
+      <c r="H46">
+        <v>32</v>
+      </c>
+      <c r="I46">
+        <v>70</v>
+      </c>
+      <c r="J46" t="s">
+        <v>18</v>
+      </c>
+      <c r="K46" t="s">
+        <v>19</v>
+      </c>
+      <c r="L46">
+        <v>0.88035804033279419</v>
+      </c>
+      <c r="M46">
+        <v>0.86099857091903687</v>
+      </c>
+      <c r="N46">
+        <v>0</v>
+      </c>
+      <c r="O46" t="s">
+        <v>21</v>
+      </c>
+      <c r="P46" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="47" spans="1:20" x14ac:dyDescent="0.3">
+      <c r="A47" t="s">
+        <v>16</v>
+      </c>
+      <c r="B47">
+        <v>9</v>
+      </c>
+      <c r="C47">
+        <v>1E-3</v>
+      </c>
+      <c r="D47">
+        <v>0</v>
+      </c>
+      <c r="E47" t="s">
+        <v>17</v>
+      </c>
+      <c r="F47">
+        <v>0</v>
+      </c>
+      <c r="G47" t="s">
+        <v>40</v>
+      </c>
+      <c r="H47">
+        <v>32</v>
+      </c>
+      <c r="I47">
+        <v>150</v>
+      </c>
+      <c r="J47" t="s">
+        <v>18</v>
+      </c>
+      <c r="K47" t="s">
+        <v>19</v>
+      </c>
+      <c r="L47">
+        <v>0.84722715616226196</v>
+      </c>
+      <c r="M47">
+        <v>0.83071082830429077</v>
+      </c>
+      <c r="N47">
+        <v>0.35570000000000002</v>
+      </c>
+      <c r="O47" t="s">
+        <v>21</v>
+      </c>
+      <c r="P47" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="48" spans="1:20" x14ac:dyDescent="0.3">
+      <c r="A48" t="s">
+        <v>16</v>
+      </c>
+      <c r="B48">
+        <v>9</v>
+      </c>
+      <c r="C48">
+        <v>1E-3</v>
+      </c>
+      <c r="D48">
+        <v>0</v>
+      </c>
+      <c r="E48" t="s">
+        <v>17</v>
+      </c>
+      <c r="F48">
+        <v>0</v>
+      </c>
+      <c r="G48" t="s">
+        <v>41</v>
+      </c>
+      <c r="H48">
+        <v>32</v>
+      </c>
+      <c r="I48">
+        <v>150</v>
+      </c>
+      <c r="J48" t="s">
+        <v>18</v>
+      </c>
+      <c r="K48" t="s">
+        <v>19</v>
+      </c>
+      <c r="L48">
+        <v>0.63301718235015869</v>
+      </c>
+      <c r="M48">
+        <v>0.6305963397026062</v>
+      </c>
+      <c r="N48">
+        <v>0.35610000000000003</v>
+      </c>
+      <c r="O48" t="s">
+        <v>21</v>
+      </c>
+      <c r="P48" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="49" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="A49" t="s">
+        <v>16</v>
+      </c>
+      <c r="B49">
+        <v>9</v>
+      </c>
+      <c r="C49">
+        <v>1E-3</v>
+      </c>
+      <c r="D49">
+        <v>0</v>
+      </c>
+      <c r="E49" t="s">
+        <v>17</v>
+      </c>
+      <c r="F49">
+        <v>0</v>
+      </c>
+      <c r="G49" t="s">
+        <v>43</v>
+      </c>
+      <c r="H49">
+        <v>32</v>
+      </c>
+      <c r="I49">
+        <v>150</v>
+      </c>
+      <c r="J49" t="s">
+        <v>18</v>
+      </c>
+      <c r="K49" t="s">
+        <v>19</v>
+      </c>
+      <c r="L49">
+        <v>0.76363092660903931</v>
+      </c>
+      <c r="M49">
+        <v>0.75494736433029175</v>
+      </c>
+      <c r="N49">
+        <v>0.3553</v>
+      </c>
+      <c r="O49" t="s">
+        <v>21</v>
+      </c>
+      <c r="P49" t="s">
         <v>22</v>
       </c>
     </row>

</xml_diff>